<commit_message>
FEAT - Projeto no intelliJ adicionado, com configrações e pacotes necessários
</commit_message>
<xml_diff>
--- a/DOCS/burndown_sprint.xlsx
+++ b/DOCS/burndown_sprint.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\FATEC\sem2\API\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\FATEC\sem2\API-2\DOCS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D84D0AEF-6AA2-4F95-8F57-09A52D45F657}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD11D96B-FD7A-49E8-8935-161490EBA35A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>Total de horas</t>
   </si>
@@ -99,77 +99,56 @@
     <t>Dia 20</t>
   </si>
   <si>
-    <t>Atividade 1</t>
-  </si>
-  <si>
-    <t>Atividade 2</t>
-  </si>
-  <si>
-    <t>Atividade 3</t>
-  </si>
-  <si>
-    <t>Atividade 4</t>
-  </si>
-  <si>
-    <t>Atividade 5</t>
-  </si>
-  <si>
-    <t>Atividade 6</t>
-  </si>
-  <si>
-    <t>Atividade 7</t>
-  </si>
-  <si>
-    <t>Atividade 8</t>
-  </si>
-  <si>
-    <t>Atividade 9</t>
-  </si>
-  <si>
-    <t>Atividade 10</t>
-  </si>
-  <si>
-    <t>Atividade 11</t>
-  </si>
-  <si>
-    <t>Atividade 12</t>
-  </si>
-  <si>
-    <t>Atividade 13</t>
-  </si>
-  <si>
-    <t>Atividade 14</t>
-  </si>
-  <si>
-    <t>Atividade 15</t>
-  </si>
-  <si>
-    <t>Atividade 16</t>
-  </si>
-  <si>
-    <t>Atividade 17</t>
-  </si>
-  <si>
-    <t>Atividade 18</t>
-  </si>
-  <si>
-    <t>Atividade 19</t>
-  </si>
-  <si>
-    <t>Atividade 20</t>
-  </si>
-  <si>
     <t>Restante</t>
   </si>
   <si>
     <t>Estimado</t>
+  </si>
+  <si>
+    <t>US-1.1</t>
+  </si>
+  <si>
+    <t>US-1.2</t>
+  </si>
+  <si>
+    <t>US-1.3</t>
+  </si>
+  <si>
+    <t>US-1.4</t>
+  </si>
+  <si>
+    <t>US-1.5</t>
+  </si>
+  <si>
+    <t>US-1.6</t>
+  </si>
+  <si>
+    <t>US-2.1</t>
+  </si>
+  <si>
+    <t>US-2.2</t>
+  </si>
+  <si>
+    <t>US-2.3</t>
+  </si>
+  <si>
+    <t>US-3.1</t>
+  </si>
+  <si>
+    <t>US-3.2</t>
+  </si>
+  <si>
+    <t>US-3.3</t>
+  </si>
+  <si>
+    <t>Coluna1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -181,6 +160,23 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -203,16 +199,455 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="24">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -230,16 +665,33 @@
   <c:date1904 val="0"/>
   <c:lang val="pt-BR"/>
   <c:roundedCorners val="1"/>
-  <c:style val="10"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
         <c:rich>
-          <a:bodyPr/>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr/>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
             </a:pPr>
             <a:r>
               <a:rPr lang="pt-BR"/>
@@ -249,6 +701,13 @@
         </c:rich>
       </c:tx>
       <c:overlay val="1"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -258,9 +717,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="1.8333333333333333E-2"/>
-          <c:y val="0.10701352027949831"/>
+          <c:y val="0.16635028614412714"/>
           <c:w val="0.96333333333333337"/>
-          <c:h val="0.8555715628089936"/>
+          <c:h val="0.69344609983479688"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -273,9 +732,19 @@
             <c:v>Restante</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
             </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="35000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
           </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
@@ -353,72 +822,72 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Burndown Chart'!$B$22:$V$22</c:f>
+              <c:f>'Burndown Chart'!$B$14:$V$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>275</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>260</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>258</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>258</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>258</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>258</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>258</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>258</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>258</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>258</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>258</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>258</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>258</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>258</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>258</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>258</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>258</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>258</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>258</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>258</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>258</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -437,9 +906,19 @@
             <c:v>Estimado</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
             </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="35000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
           </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
@@ -517,72 +996,72 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Burndown Chart'!$B$23:$V$23</c:f>
+              <c:f>'Burndown Chart'!$B$15:$V$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>275</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>261.25</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>247.5</c:v>
+                  <c:v>55.1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>233.75</c:v>
+                  <c:v>52.2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>220</c:v>
+                  <c:v>49.3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>206.25</c:v>
+                  <c:v>46.4</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>192.5</c:v>
+                  <c:v>43.5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>178.75</c:v>
+                  <c:v>40.6</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>165</c:v>
+                  <c:v>37.700000000000003</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>151.25</c:v>
+                  <c:v>34.799999999999997</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>137.5</c:v>
+                  <c:v>31.9</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>123.75</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>110</c:v>
+                  <c:v>26.1</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>96.25</c:v>
+                  <c:v>23.2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>82.5</c:v>
+                  <c:v>20.3</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>68.75</c:v>
+                  <c:v>17.399999999999999</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>55</c:v>
+                  <c:v>14.5</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>41.25</c:v>
+                  <c:v>11.6</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>27.5</c:v>
+                  <c:v>8.6999999999999993</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>13.75</c:v>
+                  <c:v>5.8</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0</c:v>
+                  <c:v>2.9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -611,12 +1090,45 @@
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="1"/>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="dd\-mm\-yyyy" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
         <c:crossAx val="100"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
@@ -629,17 +1141,40 @@
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="1"/>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:majorGridlines/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
         <c:title>
           <c:tx>
             <c:rich>
-              <a:bodyPr/>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="pt-BR"/>
@@ -649,24 +1184,117 @@
             </c:rich>
           </c:tx>
           <c:overlay val="1"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
         <c:crossAx val="500"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="1"/>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="1"/>
   </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-BR"/>
+    </a:p>
+  </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -682,21 +1310,31 @@
   <c:roundedCorners val="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="110"/>
+      <c14:style val="102"/>
     </mc:Choice>
     <mc:Fallback>
-      <c:style val="10"/>
+      <c:style val="2"/>
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
         <c:rich>
-          <a:bodyPr/>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr/>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
             </a:pPr>
             <a:r>
               <a:rPr lang="pt-BR"/>
@@ -706,6 +1344,13 @@
         </c:rich>
       </c:tx>
       <c:overlay val="1"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -715,9 +1360,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="1.8333333333333333E-2"/>
-          <c:y val="6.8027192665061686E-2"/>
+          <c:y val="0.16635028614412714"/>
           <c:w val="0.96333333333333337"/>
-          <c:h val="0.89455785136915433"/>
+          <c:h val="0.69344609983479688"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -730,9 +1375,19 @@
             <c:v>Restante</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
             </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="35000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
           </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
@@ -810,72 +1465,72 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Burndown Chart'!$B$22:$V$22</c:f>
+              <c:f>'Burndown Chart'!$B$14:$V$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>275</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>260</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>258</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>258</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>258</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>258</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>258</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>258</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>258</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>258</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>258</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>258</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>258</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>258</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>258</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>258</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>258</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>258</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>258</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>258</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>258</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -883,7 +1538,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-7ADF-4B17-B3C6-E0E59568A6C7}"/>
+              <c16:uniqueId val="{00000000-EEAE-44C0-9D20-ACFA05CAA252}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -894,9 +1549,19 @@
             <c:v>Estimado</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
             </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="35000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
           </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
@@ -974,72 +1639,72 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Burndown Chart'!$B$23:$V$23</c:f>
+              <c:f>'Burndown Chart'!$B$15:$V$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>275</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>261.25</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>247.5</c:v>
+                  <c:v>55.1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>233.75</c:v>
+                  <c:v>52.2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>220</c:v>
+                  <c:v>49.3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>206.25</c:v>
+                  <c:v>46.4</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>192.5</c:v>
+                  <c:v>43.5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>178.75</c:v>
+                  <c:v>40.6</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>165</c:v>
+                  <c:v>37.700000000000003</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>151.25</c:v>
+                  <c:v>34.799999999999997</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>137.5</c:v>
+                  <c:v>31.9</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>123.75</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>110</c:v>
+                  <c:v>26.1</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>96.25</c:v>
+                  <c:v>23.2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>82.5</c:v>
+                  <c:v>20.3</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>68.75</c:v>
+                  <c:v>17.399999999999999</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>55</c:v>
+                  <c:v>14.5</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>41.25</c:v>
+                  <c:v>11.6</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>27.5</c:v>
+                  <c:v>8.6999999999999993</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>13.75</c:v>
+                  <c:v>5.8</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0</c:v>
+                  <c:v>2.9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1047,12 +1712,11 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-7ADF-4B17-B3C6-E0E59568A6C7}"/>
+              <c16:uniqueId val="{00000001-EEAE-44C0-9D20-ACFA05CAA252}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -1072,9 +1736,42 @@
         <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="dd\-mm\-yyyy" sourceLinked="0"/>
-        <c:majorTickMark val="out"/>
+        <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
         <c:crossAx val="100"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
@@ -1089,15 +1786,38 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:majorGridlines/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
         <c:title>
           <c:tx>
             <c:rich>
-              <a:bodyPr/>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="pt-BR"/>
@@ -1107,24 +1827,117 @@
             </c:rich>
           </c:tx>
           <c:overlay val="1"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
+        <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
         <c:crossAx val="500"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="1"/>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="1"/>
   </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-BR"/>
+    </a:p>
+  </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -1137,12 +1950,12 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>76199</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="3981450" cy="3257551"/>
+    <xdr:ext cx="6191250" cy="3638551"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -1174,17 +1987,17 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>66675</xdr:colOff>
+      <xdr:colOff>219075</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:rowOff>133351</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="11239500" cy="5991225"/>
+    <xdr:ext cx="14430375" cy="5829299"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
+        <xdr:cNvPr id="3" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3C394049-F161-4CD6-B51C-CA4EE50A1823}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{54E86CFF-85C4-4865-AED4-CCDE7758226C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1205,6 +2018,37 @@
     <xdr:clientData/>
   </xdr:oneCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E1884C1C-B0F0-42C1-9734-A26A7C746AC5}" name="Tabela2" displayName="Tabela2" ref="A1:V15" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
+  <autoFilter ref="A1:V15" xr:uid="{E1884C1C-B0F0-42C1-9734-A26A7C746AC5}"/>
+  <tableColumns count="22">
+    <tableColumn id="1" xr3:uid="{DC2BAE98-3A26-4BC7-8ED6-C3303DF0038D}" name="Coluna1" dataDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{1A2025CD-23B1-415B-92B3-5881DCA18C20}" name="Total de horas" dataDxfId="20"/>
+    <tableColumn id="3" xr3:uid="{4BC0BD76-7741-45BB-97A7-D6882CC1F1D8}" name="Dia 1" dataDxfId="19"/>
+    <tableColumn id="4" xr3:uid="{00882AA1-DD73-47DC-8C10-EF217AC99768}" name="Dia 2" dataDxfId="18"/>
+    <tableColumn id="5" xr3:uid="{26CA22D1-FC01-468E-9640-E8C45E991335}" name="Dia 3" dataDxfId="17"/>
+    <tableColumn id="6" xr3:uid="{8637A8CA-1019-4007-B1C8-E2B239B9DDE1}" name="Dia 4" dataDxfId="16"/>
+    <tableColumn id="7" xr3:uid="{A817E580-DFE5-4C0E-95B3-BA357CCF9AE1}" name="Dia 5" dataDxfId="15"/>
+    <tableColumn id="8" xr3:uid="{D4E45274-3E12-45D7-8440-09BF785A95E4}" name="Dia 6" dataDxfId="14"/>
+    <tableColumn id="9" xr3:uid="{731C7356-2D40-41A5-B847-23C816E5BAD2}" name="Dia 7" dataDxfId="13"/>
+    <tableColumn id="10" xr3:uid="{824F84C5-6311-4AAA-96D8-D8FD71FBBAF6}" name="Dia 8" dataDxfId="12"/>
+    <tableColumn id="11" xr3:uid="{A41E8023-6BEE-4187-9A47-DA4E41991646}" name="Dia 9" dataDxfId="11"/>
+    <tableColumn id="12" xr3:uid="{FCCE3901-00D6-4E75-A167-FD4C20E71CF2}" name="Dia 10" dataDxfId="10"/>
+    <tableColumn id="13" xr3:uid="{E9D6ACAB-EF0B-42EB-977B-E157431B7C93}" name="Dia 11" dataDxfId="9"/>
+    <tableColumn id="14" xr3:uid="{7DE82C8F-4251-435F-8119-4098379E7C92}" name="Dia 12" dataDxfId="8"/>
+    <tableColumn id="15" xr3:uid="{C0057573-93FA-4291-8B0E-84DA468004AA}" name="Dia 13" dataDxfId="7"/>
+    <tableColumn id="16" xr3:uid="{616A7614-87CD-480E-8FB6-B3E991E2E773}" name="Dia 14" dataDxfId="6"/>
+    <tableColumn id="17" xr3:uid="{1EA39BE6-7D7D-43AD-8119-68FE10A2BB9C}" name="Dia 15" dataDxfId="5"/>
+    <tableColumn id="18" xr3:uid="{EF7A01F8-F878-4FFE-B140-126C702615BE}" name="Dia 16" dataDxfId="4"/>
+    <tableColumn id="19" xr3:uid="{9701BAD2-120F-49E8-9004-331E6F9C2716}" name="Dia 17" dataDxfId="3"/>
+    <tableColumn id="20" xr3:uid="{72A17F3E-6229-46C9-8FEE-BDF8B519F9FD}" name="Dia 18" dataDxfId="2"/>
+    <tableColumn id="21" xr3:uid="{1C3259A9-A4D5-488F-BE54-1D541CFA2C96}" name="Dia 19" dataDxfId="1"/>
+    <tableColumn id="22" xr3:uid="{4411E0A4-16AB-46BD-886B-34DA12503542}" name="Dia 20" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1492,16 +2336,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V23"/>
+  <dimension ref="A1:V21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Y3" sqref="Y3"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="11" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="21" width="10.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A1" s="1"/>
+      <c r="A1" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1567,15 +2420,13 @@
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>21</v>
+      <c r="A2" s="3" t="s">
+        <v>23</v>
       </c>
       <c r="B2" s="1">
-        <v>20</v>
-      </c>
-      <c r="C2" s="1">
-        <v>10</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
@@ -1598,14 +2449,12 @@
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B3" s="1">
-        <v>10</v>
-      </c>
-      <c r="C3" s="1">
-        <v>5</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
@@ -1628,15 +2477,13 @@
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B4" s="1">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="C4" s="1"/>
-      <c r="D4" s="1">
-        <v>2</v>
-      </c>
+      <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
@@ -1658,10 +2505,10 @@
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B5" s="1">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -1686,10 +2533,10 @@
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B6" s="1">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -1714,10 +2561,10 @@
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B7" s="1">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -1742,10 +2589,10 @@
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B8" s="1">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -1770,10 +2617,10 @@
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B9" s="1">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -1798,10 +2645,10 @@
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B10" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -1826,10 +2673,10 @@
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B11" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
@@ -1854,10 +2701,10 @@
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B12" s="1">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
@@ -1882,10 +2729,10 @@
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B13" s="1">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -1910,67 +2757,164 @@
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="B14" s="1">
-        <v>13</v>
-      </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
-      <c r="K14" s="1"/>
-      <c r="L14" s="1"/>
-      <c r="M14" s="1"/>
-      <c r="N14" s="1"/>
-      <c r="O14" s="1"/>
-      <c r="P14" s="1"/>
-      <c r="Q14" s="1"/>
-      <c r="R14" s="1"/>
-      <c r="S14" s="1"/>
-      <c r="T14" s="1"/>
-      <c r="U14" s="1"/>
-      <c r="V14" s="1"/>
+        <v>58</v>
+      </c>
+      <c r="C14" s="1">
+        <f>B14-SUM(C2:C13)</f>
+        <v>58</v>
+      </c>
+      <c r="D14" s="1">
+        <f t="shared" ref="D14:V14" si="0">C14-SUM(D2:D13)</f>
+        <v>58</v>
+      </c>
+      <c r="E14" s="1">
+        <f t="shared" si="0"/>
+        <v>58</v>
+      </c>
+      <c r="F14" s="1">
+        <f t="shared" si="0"/>
+        <v>58</v>
+      </c>
+      <c r="G14" s="1">
+        <f t="shared" si="0"/>
+        <v>58</v>
+      </c>
+      <c r="H14" s="1">
+        <f t="shared" si="0"/>
+        <v>58</v>
+      </c>
+      <c r="I14" s="1">
+        <f t="shared" si="0"/>
+        <v>58</v>
+      </c>
+      <c r="J14" s="1">
+        <f t="shared" si="0"/>
+        <v>58</v>
+      </c>
+      <c r="K14" s="1">
+        <f t="shared" si="0"/>
+        <v>58</v>
+      </c>
+      <c r="L14" s="1">
+        <f t="shared" si="0"/>
+        <v>58</v>
+      </c>
+      <c r="M14" s="1">
+        <f t="shared" si="0"/>
+        <v>58</v>
+      </c>
+      <c r="N14" s="1">
+        <f t="shared" si="0"/>
+        <v>58</v>
+      </c>
+      <c r="O14" s="1">
+        <f t="shared" si="0"/>
+        <v>58</v>
+      </c>
+      <c r="P14" s="1">
+        <f t="shared" si="0"/>
+        <v>58</v>
+      </c>
+      <c r="Q14" s="1">
+        <f t="shared" si="0"/>
+        <v>58</v>
+      </c>
+      <c r="R14" s="1">
+        <f t="shared" si="0"/>
+        <v>58</v>
+      </c>
+      <c r="S14" s="1">
+        <f t="shared" si="0"/>
+        <v>58</v>
+      </c>
+      <c r="T14" s="1">
+        <f t="shared" si="0"/>
+        <v>58</v>
+      </c>
+      <c r="U14" s="1">
+        <f t="shared" si="0"/>
+        <v>58</v>
+      </c>
+      <c r="V14" s="1">
+        <f t="shared" si="0"/>
+        <v>58</v>
+      </c>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="B15" s="1">
-        <v>14</v>
-      </c>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
-      <c r="K15" s="1"/>
-      <c r="L15" s="1"/>
-      <c r="M15" s="1"/>
-      <c r="N15" s="1"/>
-      <c r="O15" s="1"/>
-      <c r="P15" s="1"/>
-      <c r="Q15" s="1"/>
-      <c r="R15" s="1"/>
-      <c r="S15" s="1"/>
-      <c r="T15" s="1"/>
-      <c r="U15" s="1"/>
-      <c r="V15" s="1"/>
+        <f>SUM(B2:B13)</f>
+        <v>58</v>
+      </c>
+      <c r="C15" s="1">
+        <v>58</v>
+      </c>
+      <c r="D15" s="1">
+        <v>55.1</v>
+      </c>
+      <c r="E15" s="1">
+        <v>52.2</v>
+      </c>
+      <c r="F15" s="1">
+        <v>49.3</v>
+      </c>
+      <c r="G15" s="1">
+        <v>46.4</v>
+      </c>
+      <c r="H15" s="1">
+        <v>43.5</v>
+      </c>
+      <c r="I15" s="1">
+        <v>40.6</v>
+      </c>
+      <c r="J15" s="1">
+        <v>37.700000000000003</v>
+      </c>
+      <c r="K15" s="1">
+        <v>34.799999999999997</v>
+      </c>
+      <c r="L15" s="1">
+        <v>31.9</v>
+      </c>
+      <c r="M15" s="1">
+        <v>29</v>
+      </c>
+      <c r="N15" s="1">
+        <v>26.1</v>
+      </c>
+      <c r="O15" s="1">
+        <v>23.2</v>
+      </c>
+      <c r="P15" s="1">
+        <v>20.3</v>
+      </c>
+      <c r="Q15" s="1">
+        <v>17.399999999999999</v>
+      </c>
+      <c r="R15" s="1">
+        <v>14.5</v>
+      </c>
+      <c r="S15" s="1">
+        <v>11.6</v>
+      </c>
+      <c r="T15" s="1">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="U15" s="1">
+        <v>5.8</v>
+      </c>
+      <c r="V15" s="1">
+        <v>2.9</v>
+      </c>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B16" s="1">
-        <v>15</v>
-      </c>
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
@@ -1993,12 +2937,8 @@
       <c r="V16" s="1"/>
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B17" s="1">
-        <v>16</v>
-      </c>
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
@@ -2021,12 +2961,8 @@
       <c r="V17" s="1"/>
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B18" s="1">
-        <v>17</v>
-      </c>
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
@@ -2049,12 +2985,8 @@
       <c r="V18" s="1"/>
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B19" s="1">
-        <v>18</v>
-      </c>
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
@@ -2077,12 +3009,8 @@
       <c r="V19" s="1"/>
     </row>
     <row r="20" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B20" s="1">
-        <v>19</v>
-      </c>
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
@@ -2105,12 +3033,8 @@
       <c r="V20" s="1"/>
     </row>
     <row r="21" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B21" s="1">
-        <v>20</v>
-      </c>
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
@@ -2120,7 +3044,7 @@
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
-      <c r="L21" s="1"/>
+      <c r="L21" s="2"/>
       <c r="M21" s="1"/>
       <c r="N21" s="1"/>
       <c r="O21" s="1"/>
@@ -2132,165 +3056,13 @@
       <c r="U21" s="1"/>
       <c r="V21" s="1"/>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B22" s="1">
-        <v>275</v>
-      </c>
-      <c r="C22" s="1">
-        <f t="shared" ref="C22:V22" si="0">B22-SUM(C2:C21)</f>
-        <v>260</v>
-      </c>
-      <c r="D22" s="1">
-        <f t="shared" si="0"/>
-        <v>258</v>
-      </c>
-      <c r="E22" s="1">
-        <f t="shared" si="0"/>
-        <v>258</v>
-      </c>
-      <c r="F22" s="1">
-        <f t="shared" si="0"/>
-        <v>258</v>
-      </c>
-      <c r="G22" s="1">
-        <f t="shared" si="0"/>
-        <v>258</v>
-      </c>
-      <c r="H22" s="1">
-        <f t="shared" si="0"/>
-        <v>258</v>
-      </c>
-      <c r="I22" s="1">
-        <f t="shared" si="0"/>
-        <v>258</v>
-      </c>
-      <c r="J22" s="1">
-        <f t="shared" si="0"/>
-        <v>258</v>
-      </c>
-      <c r="K22" s="1">
-        <f t="shared" si="0"/>
-        <v>258</v>
-      </c>
-      <c r="L22" s="1">
-        <f t="shared" si="0"/>
-        <v>258</v>
-      </c>
-      <c r="M22" s="1">
-        <f t="shared" si="0"/>
-        <v>258</v>
-      </c>
-      <c r="N22" s="1">
-        <f t="shared" si="0"/>
-        <v>258</v>
-      </c>
-      <c r="O22" s="1">
-        <f t="shared" si="0"/>
-        <v>258</v>
-      </c>
-      <c r="P22" s="1">
-        <f t="shared" si="0"/>
-        <v>258</v>
-      </c>
-      <c r="Q22" s="1">
-        <f t="shared" si="0"/>
-        <v>258</v>
-      </c>
-      <c r="R22" s="1">
-        <f t="shared" si="0"/>
-        <v>258</v>
-      </c>
-      <c r="S22" s="1">
-        <f t="shared" si="0"/>
-        <v>258</v>
-      </c>
-      <c r="T22" s="1">
-        <f t="shared" si="0"/>
-        <v>258</v>
-      </c>
-      <c r="U22" s="1">
-        <f t="shared" si="0"/>
-        <v>258</v>
-      </c>
-      <c r="V22" s="1">
-        <f t="shared" si="0"/>
-        <v>258</v>
-      </c>
-    </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B23" s="1">
-        <v>275</v>
-      </c>
-      <c r="C23" s="1">
-        <v>261.25</v>
-      </c>
-      <c r="D23" s="1">
-        <v>247.5</v>
-      </c>
-      <c r="E23" s="1">
-        <v>233.75</v>
-      </c>
-      <c r="F23" s="1">
-        <v>220</v>
-      </c>
-      <c r="G23" s="1">
-        <v>206.25</v>
-      </c>
-      <c r="H23" s="1">
-        <v>192.5</v>
-      </c>
-      <c r="I23" s="1">
-        <v>178.75</v>
-      </c>
-      <c r="J23" s="1">
-        <v>165</v>
-      </c>
-      <c r="K23" s="1">
-        <v>151.25</v>
-      </c>
-      <c r="L23" s="1">
-        <v>137.5</v>
-      </c>
-      <c r="M23" s="1">
-        <v>123.75</v>
-      </c>
-      <c r="N23" s="1">
-        <v>110</v>
-      </c>
-      <c r="O23" s="1">
-        <v>96.25</v>
-      </c>
-      <c r="P23" s="1">
-        <v>82.5</v>
-      </c>
-      <c r="Q23" s="1">
-        <v>68.75</v>
-      </c>
-      <c r="R23" s="1">
-        <v>55</v>
-      </c>
-      <c r="S23" s="1">
-        <v>41.25</v>
-      </c>
-      <c r="T23" s="1">
-        <v>27.5</v>
-      </c>
-      <c r="U23" s="1">
-        <v>13.75</v>
-      </c>
-      <c r="V23" s="1">
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -2298,8 +3070,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7AEF5D5-9845-4510-B31C-B45C1A0563CA}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="U17" sqref="U17"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="S33" sqref="S33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
FEAT - Adicionada a classe Cliente com atributos e métodos básicos DOCS - banco de dados, diagrama de banco de dados
</commit_message>
<xml_diff>
--- a/DOCS/burndown_sprint.xlsx
+++ b/DOCS/burndown_sprint.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\FATEC\sem2\API-2\DOCS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD11D96B-FD7A-49E8-8935-161490EBA35A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B96FC6C-C3A7-40FC-963C-BA2189A5E648}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -848,46 +848,46 @@
                   <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>58</c:v>
+                  <c:v>53.5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>58</c:v>
+                  <c:v>51</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>58</c:v>
+                  <c:v>46</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>58</c:v>
+                  <c:v>46</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>58</c:v>
+                  <c:v>46</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>58</c:v>
+                  <c:v>46</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>58</c:v>
+                  <c:v>46</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>58</c:v>
+                  <c:v>46</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>58</c:v>
+                  <c:v>46</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>58</c:v>
+                  <c:v>46</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>58</c:v>
+                  <c:v>46</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>58</c:v>
+                  <c:v>46</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>58</c:v>
+                  <c:v>46</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>58</c:v>
+                  <c:v>46</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1491,46 +1491,46 @@
                   <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>58</c:v>
+                  <c:v>53.5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>58</c:v>
+                  <c:v>51</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>58</c:v>
+                  <c:v>46</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>58</c:v>
+                  <c:v>46</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>58</c:v>
+                  <c:v>46</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>58</c:v>
+                  <c:v>46</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>58</c:v>
+                  <c:v>46</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>58</c:v>
+                  <c:v>46</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>58</c:v>
+                  <c:v>46</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>58</c:v>
+                  <c:v>46</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>58</c:v>
+                  <c:v>46</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>58</c:v>
+                  <c:v>46</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>58</c:v>
+                  <c:v>46</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>58</c:v>
+                  <c:v>46</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2339,7 +2339,7 @@
   <dimension ref="A1:V21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2462,7 +2462,9 @@
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
+      <c r="K3" s="1">
+        <v>2</v>
+      </c>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
@@ -2490,7 +2492,9 @@
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
+      <c r="K4" s="1">
+        <v>3</v>
+      </c>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
@@ -2544,7 +2548,9 @@
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
+      <c r="I6" s="1">
+        <v>1</v>
+      </c>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
@@ -2628,8 +2634,12 @@
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
+      <c r="I9" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="J9" s="3">
+        <v>1.5</v>
+      </c>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
@@ -2657,7 +2667,9 @@
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
+      <c r="J10" s="1">
+        <v>1</v>
+      </c>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
@@ -2684,7 +2696,9 @@
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
+      <c r="I11" s="1">
+        <v>2</v>
+      </c>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
@@ -2788,59 +2802,59 @@
       </c>
       <c r="I14" s="1">
         <f t="shared" si="0"/>
-        <v>58</v>
+        <v>53.5</v>
       </c>
       <c r="J14" s="1">
         <f t="shared" si="0"/>
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="K14" s="1">
         <f t="shared" si="0"/>
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="L14" s="1">
         <f t="shared" si="0"/>
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="M14" s="1">
         <f t="shared" si="0"/>
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="N14" s="1">
         <f t="shared" si="0"/>
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="O14" s="1">
         <f t="shared" si="0"/>
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="P14" s="1">
         <f t="shared" si="0"/>
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="Q14" s="1">
         <f t="shared" si="0"/>
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="R14" s="1">
         <f t="shared" si="0"/>
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="S14" s="1">
         <f t="shared" si="0"/>
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="T14" s="1">
         <f t="shared" si="0"/>
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="U14" s="1">
         <f t="shared" si="0"/>
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="V14" s="1">
         <f t="shared" si="0"/>
-        <v>58</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
DOCS - product backlog table
</commit_message>
<xml_diff>
--- a/DOCS/burndown_sprint.xlsx
+++ b/DOCS/burndown_sprint.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\FATEC\sem2\API-2\DOCS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B96FC6C-C3A7-40FC-963C-BA2189A5E648}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B431E395-FF05-42FC-B301-B77283407DAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t>Total de horas</t>
   </si>
@@ -105,50 +105,71 @@
     <t>Estimado</t>
   </si>
   <si>
-    <t>US-1.1</t>
-  </si>
-  <si>
-    <t>US-1.2</t>
-  </si>
-  <si>
-    <t>US-1.3</t>
-  </si>
-  <si>
-    <t>US-1.4</t>
-  </si>
-  <si>
-    <t>US-1.5</t>
-  </si>
-  <si>
-    <t>US-1.6</t>
-  </si>
-  <si>
-    <t>US-2.1</t>
-  </si>
-  <si>
-    <t>US-2.2</t>
-  </si>
-  <si>
-    <t>US-2.3</t>
-  </si>
-  <si>
-    <t>US-3.1</t>
-  </si>
-  <si>
-    <t>US-3.2</t>
-  </si>
-  <si>
-    <t>US-3.3</t>
-  </si>
-  <si>
-    <t>Coluna1</t>
+    <t>US-1.2 (estudo)</t>
+  </si>
+  <si>
+    <t>US-1.3 (estudo)</t>
+  </si>
+  <si>
+    <t>US-1.5 (estudo)</t>
+  </si>
+  <si>
+    <t>US-2.2 (estudo)</t>
+  </si>
+  <si>
+    <t>US-3.1 (estudo)</t>
+  </si>
+  <si>
+    <t>Documentação</t>
+  </si>
+  <si>
+    <t>Tasks</t>
+  </si>
+  <si>
+    <t>US-2.1 (Banco)</t>
+  </si>
+  <si>
+    <t>US-3.3 (Testes)</t>
+  </si>
+  <si>
+    <t>US-1.6 (Testes)</t>
+  </si>
+  <si>
+    <t>US-1.1 (Banco)</t>
+  </si>
+  <si>
+    <t>US-1.4 (gabriel, front)</t>
+  </si>
+  <si>
+    <t>US-1.5 (giovanni, front)</t>
+  </si>
+  <si>
+    <t>US-2.3 (giovanni, front)</t>
+  </si>
+  <si>
+    <t>US-3.2 (gabriel, front)</t>
+  </si>
+  <si>
+    <t>US-3.1 (daniel, back)</t>
+  </si>
+  <si>
+    <t>US-2.2 (bueno, back)</t>
+  </si>
+  <si>
+    <t>US-1.7 (caio, back)</t>
+  </si>
+  <si>
+    <t>US-1.3 (monteiro, back)</t>
+  </si>
+  <si>
+    <t>US-1.2 (caio, back)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -168,26 +189,33 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor theme="4" tint="0.59999389629810485"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -195,11 +223,63 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -207,7 +287,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -822,72 +911,72 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Burndown Chart'!$B$14:$V$14</c:f>
+              <c:f>'Burndown Chart'!$B$25:$V$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>58</c:v>
+                  <c:v>86</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>58</c:v>
+                  <c:v>86</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>58</c:v>
+                  <c:v>85</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>58</c:v>
+                  <c:v>85</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>58</c:v>
+                  <c:v>84</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>58</c:v>
+                  <c:v>83</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>58</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>53.5</c:v>
+                  <c:v>71</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>51</c:v>
+                  <c:v>62</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>46</c:v>
+                  <c:v>55</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>46</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>46</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>46</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>46</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>46</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>46</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>46</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>46</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>46</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>46</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>46</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -996,72 +1085,72 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Burndown Chart'!$B$15:$V$15</c:f>
+              <c:f>'Burndown Chart'!$B$26:$V$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>58</c:v>
+                  <c:v>86</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>58</c:v>
+                  <c:v>81.7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>55.1</c:v>
+                  <c:v>77.400000000000006</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>52.2</c:v>
+                  <c:v>73.099999999999994</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>49.3</c:v>
+                  <c:v>68.8</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>46.4</c:v>
+                  <c:v>64.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43.5</c:v>
+                  <c:v>60.2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>40.6</c:v>
+                  <c:v>55.9</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>37.700000000000003</c:v>
+                  <c:v>51.6</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>34.799999999999997</c:v>
+                  <c:v>47.3</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>31.9</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>29</c:v>
+                  <c:v>38.700000000000003</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>26.1</c:v>
+                  <c:v>34.4</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>23.2</c:v>
+                  <c:v>30.1</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>20.3</c:v>
+                  <c:v>25.8</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>17.399999999999999</c:v>
+                  <c:v>21.5</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>14.5</c:v>
+                  <c:v>17.2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>11.6</c:v>
+                  <c:v>12.9</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>8.6999999999999993</c:v>
+                  <c:v>8.6000000000000902</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>5.8</c:v>
+                  <c:v>4.3000000000001002</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2.9</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1465,72 +1554,72 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Burndown Chart'!$B$14:$V$14</c:f>
+              <c:f>'Burndown Chart'!$B$25:$V$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>58</c:v>
+                  <c:v>86</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>58</c:v>
+                  <c:v>86</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>58</c:v>
+                  <c:v>85</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>58</c:v>
+                  <c:v>85</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>58</c:v>
+                  <c:v>84</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>58</c:v>
+                  <c:v>83</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>58</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>53.5</c:v>
+                  <c:v>71</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>51</c:v>
+                  <c:v>62</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>46</c:v>
+                  <c:v>55</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>46</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>46</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>46</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>46</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>46</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>46</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>46</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>46</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>46</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>46</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>46</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1639,72 +1728,72 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Burndown Chart'!$B$15:$V$15</c:f>
+              <c:f>'Burndown Chart'!$B$26:$V$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>58</c:v>
+                  <c:v>86</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>58</c:v>
+                  <c:v>81.7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>55.1</c:v>
+                  <c:v>77.400000000000006</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>52.2</c:v>
+                  <c:v>73.099999999999994</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>49.3</c:v>
+                  <c:v>68.8</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>46.4</c:v>
+                  <c:v>64.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43.5</c:v>
+                  <c:v>60.2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>40.6</c:v>
+                  <c:v>55.9</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>37.700000000000003</c:v>
+                  <c:v>51.6</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>34.799999999999997</c:v>
+                  <c:v>47.3</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>31.9</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>29</c:v>
+                  <c:v>38.700000000000003</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>26.1</c:v>
+                  <c:v>34.4</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>23.2</c:v>
+                  <c:v>30.1</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>20.3</c:v>
+                  <c:v>25.8</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>17.399999999999999</c:v>
+                  <c:v>21.5</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>14.5</c:v>
+                  <c:v>17.2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>11.6</c:v>
+                  <c:v>12.9</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>8.6999999999999993</c:v>
+                  <c:v>8.6000000000000902</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>5.8</c:v>
+                  <c:v>4.3000000000001002</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2.9</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1950,10 +2039,10 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>390524</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>14287</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="6191250" cy="3638551"/>
     <xdr:graphicFrame macro="">
@@ -2021,10 +2110,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E1884C1C-B0F0-42C1-9734-A26A7C746AC5}" name="Tabela2" displayName="Tabela2" ref="A1:V15" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
-  <autoFilter ref="A1:V15" xr:uid="{E1884C1C-B0F0-42C1-9734-A26A7C746AC5}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E1884C1C-B0F0-42C1-9734-A26A7C746AC5}" name="Tabela2" displayName="Tabela2" ref="A1:V24" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
+  <autoFilter ref="A1:V24" xr:uid="{E1884C1C-B0F0-42C1-9734-A26A7C746AC5}"/>
   <tableColumns count="22">
-    <tableColumn id="1" xr3:uid="{DC2BAE98-3A26-4BC7-8ED6-C3303DF0038D}" name="Coluna1" dataDxfId="21"/>
+    <tableColumn id="1" xr3:uid="{DC2BAE98-3A26-4BC7-8ED6-C3303DF0038D}" name="Tasks" dataDxfId="21"/>
     <tableColumn id="2" xr3:uid="{1A2025CD-23B1-415B-92B3-5881DCA18C20}" name="Total de horas" dataDxfId="20"/>
     <tableColumn id="3" xr3:uid="{4BC0BD76-7741-45BB-97A7-D6882CC1F1D8}" name="Dia 1" dataDxfId="19"/>
     <tableColumn id="4" xr3:uid="{00882AA1-DD73-47DC-8C10-EF217AC99768}" name="Dia 2" dataDxfId="18"/>
@@ -2336,15 +2425,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V21"/>
+  <dimension ref="A1:V26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q21" sqref="Q21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="11" width="9.85546875" bestFit="1" customWidth="1"/>
@@ -2352,8 +2441,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>35</v>
+      <c r="A1" s="2" t="s">
+        <v>29</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -2420,8 +2509,8 @@
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>23</v>
+      <c r="A2" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
@@ -2431,7 +2520,9 @@
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
+      <c r="H2" s="1">
+        <v>1</v>
+      </c>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
@@ -2449,7 +2540,7 @@
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="B3" s="1">
         <v>1</v>
@@ -2459,12 +2550,12 @@
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
+      <c r="H3" s="1">
+        <v>1</v>
+      </c>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
-      <c r="K3" s="1">
-        <v>2</v>
-      </c>
+      <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
@@ -2478,11 +2569,11 @@
       <c r="V3" s="1"/>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>25</v>
+      <c r="A4" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="B4" s="1">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -2493,13 +2584,15 @@
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
-      <c r="P4" s="1"/>
+      <c r="P4" s="1">
+        <v>1</v>
+      </c>
       <c r="Q4" s="1"/>
       <c r="R4" s="1"/>
       <c r="S4" s="1"/>
@@ -2509,10 +2602,10 @@
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B5" s="1">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -2536,11 +2629,11 @@
       <c r="V5" s="1"/>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>27</v>
+      <c r="A6" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="B6" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -2548,11 +2641,11 @@
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
-      <c r="I6" s="1">
-        <v>1</v>
-      </c>
+      <c r="I6" s="1"/>
       <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
+      <c r="K6" s="1">
+        <v>2</v>
+      </c>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
@@ -2566,11 +2659,11 @@
       <c r="V6" s="1"/>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>28</v>
+      <c r="A7" s="2" t="s">
+        <v>41</v>
       </c>
       <c r="B7" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -2580,8 +2673,12 @@
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
+      <c r="K7" s="1">
+        <v>3</v>
+      </c>
+      <c r="L7" s="1">
+        <v>2</v>
+      </c>
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
@@ -2594,8 +2691,8 @@
       <c r="V7" s="1"/>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>29</v>
+      <c r="A8" s="2" t="s">
+        <v>40</v>
       </c>
       <c r="B8" s="1">
         <v>3</v>
@@ -2611,7 +2708,9 @@
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
-      <c r="N8" s="1"/>
+      <c r="N8" s="1">
+        <v>3</v>
+      </c>
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
       <c r="Q8" s="1"/>
@@ -2622,11 +2721,11 @@
       <c r="V8" s="1"/>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>30</v>
+      <c r="A9" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="B9" s="1">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -2634,15 +2733,15 @@
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
-      <c r="I9" s="3">
-        <v>1.5</v>
-      </c>
-      <c r="J9" s="3">
-        <v>1.5</v>
-      </c>
+      <c r="I9" s="1">
+        <v>1</v>
+      </c>
+      <c r="J9" s="1"/>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
-      <c r="M9" s="1"/>
+      <c r="M9" s="1">
+        <v>2</v>
+      </c>
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
@@ -2654,11 +2753,11 @@
       <c r="V9" s="1"/>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>31</v>
+      <c r="A10" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="B10" s="1">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -2666,12 +2765,14 @@
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1">
-        <v>1</v>
-      </c>
+      <c r="I10" s="1">
+        <v>2</v>
+      </c>
+      <c r="J10" s="1"/>
       <c r="K10" s="1"/>
-      <c r="L10" s="1"/>
+      <c r="L10" s="1">
+        <v>3</v>
+      </c>
       <c r="M10" s="1"/>
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
@@ -2684,11 +2785,11 @@
       <c r="V10" s="1"/>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>32</v>
+      <c r="A11" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="B11" s="1">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
@@ -2696,12 +2797,12 @@
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
-      <c r="I11" s="1">
-        <v>2</v>
-      </c>
+      <c r="I11" s="1"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
-      <c r="L11" s="1"/>
+      <c r="L11" s="1">
+        <v>1</v>
+      </c>
       <c r="M11" s="1"/>
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
@@ -2714,8 +2815,8 @@
       <c r="V11" s="1"/>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>33</v>
+      <c r="A12" s="2" t="s">
+        <v>35</v>
       </c>
       <c r="B12" s="1">
         <v>8</v>
@@ -2742,11 +2843,11 @@
       <c r="V12" s="1"/>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>34</v>
+      <c r="A13" s="2" t="s">
+        <v>36</v>
       </c>
       <c r="B13" s="1">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -2755,7 +2856,9 @@
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
+      <c r="J13" s="1">
+        <v>1</v>
+      </c>
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
@@ -2770,173 +2873,90 @@
       <c r="V13" s="1"/>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>21</v>
+      <c r="A14" s="2" t="s">
+        <v>37</v>
       </c>
       <c r="B14" s="1">
-        <v>58</v>
-      </c>
-      <c r="C14" s="1">
-        <f>B14-SUM(C2:C13)</f>
-        <v>58</v>
-      </c>
-      <c r="D14" s="1">
-        <f t="shared" ref="D14:V14" si="0">C14-SUM(D2:D13)</f>
-        <v>58</v>
-      </c>
-      <c r="E14" s="1">
-        <f t="shared" si="0"/>
-        <v>58</v>
-      </c>
-      <c r="F14" s="1">
-        <f t="shared" si="0"/>
-        <v>58</v>
-      </c>
-      <c r="G14" s="1">
-        <f t="shared" si="0"/>
-        <v>58</v>
-      </c>
-      <c r="H14" s="1">
-        <f t="shared" si="0"/>
-        <v>58</v>
-      </c>
-      <c r="I14" s="1">
-        <f t="shared" si="0"/>
-        <v>53.5</v>
-      </c>
-      <c r="J14" s="1">
-        <f t="shared" si="0"/>
-        <v>51</v>
-      </c>
-      <c r="K14" s="1">
-        <f t="shared" si="0"/>
-        <v>46</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
       <c r="L14" s="1">
-        <f t="shared" si="0"/>
-        <v>46</v>
+        <v>1</v>
       </c>
       <c r="M14" s="1">
-        <f t="shared" si="0"/>
-        <v>46</v>
-      </c>
-      <c r="N14" s="1">
-        <f t="shared" si="0"/>
-        <v>46</v>
-      </c>
-      <c r="O14" s="1">
-        <f t="shared" si="0"/>
-        <v>46</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
       <c r="P14" s="1">
-        <f t="shared" si="0"/>
-        <v>46</v>
-      </c>
-      <c r="Q14" s="1">
-        <f t="shared" si="0"/>
-        <v>46</v>
-      </c>
-      <c r="R14" s="1">
-        <f t="shared" si="0"/>
-        <v>46</v>
-      </c>
-      <c r="S14" s="1">
-        <f t="shared" si="0"/>
-        <v>46</v>
-      </c>
-      <c r="T14" s="1">
-        <f t="shared" si="0"/>
-        <v>46</v>
-      </c>
-      <c r="U14" s="1">
-        <f t="shared" si="0"/>
-        <v>46</v>
-      </c>
-      <c r="V14" s="1">
-        <f t="shared" si="0"/>
-        <v>46</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="Q14" s="1"/>
+      <c r="R14" s="1"/>
+      <c r="S14" s="1"/>
+      <c r="T14" s="1"/>
+      <c r="U14" s="1"/>
+      <c r="V14" s="1"/>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B15" s="1">
-        <f>SUM(B2:B13)</f>
-        <v>58</v>
-      </c>
-      <c r="C15" s="1">
-        <v>58</v>
-      </c>
-      <c r="D15" s="1">
-        <v>55.1</v>
-      </c>
-      <c r="E15" s="1">
-        <v>52.2</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
       <c r="F15" s="1">
-        <v>49.3</v>
-      </c>
-      <c r="G15" s="1">
-        <v>46.4</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="G15" s="1"/>
       <c r="H15" s="1">
-        <v>43.5</v>
-      </c>
-      <c r="I15" s="1">
-        <v>40.6</v>
-      </c>
-      <c r="J15" s="1">
-        <v>37.700000000000003</v>
-      </c>
-      <c r="K15" s="1">
-        <v>34.799999999999997</v>
-      </c>
-      <c r="L15" s="1">
-        <v>31.9</v>
-      </c>
-      <c r="M15" s="1">
-        <v>29</v>
-      </c>
-      <c r="N15" s="1">
-        <v>26.1</v>
-      </c>
-      <c r="O15" s="1">
-        <v>23.2</v>
-      </c>
-      <c r="P15" s="1">
-        <v>20.3</v>
-      </c>
-      <c r="Q15" s="1">
-        <v>17.399999999999999</v>
-      </c>
-      <c r="R15" s="1">
-        <v>14.5</v>
-      </c>
-      <c r="S15" s="1">
-        <v>11.6</v>
-      </c>
-      <c r="T15" s="1">
-        <v>8.6999999999999993</v>
-      </c>
-      <c r="U15" s="1">
-        <v>5.8</v>
-      </c>
-      <c r="V15" s="1">
-        <v>2.9</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
+      <c r="Q15" s="1"/>
+      <c r="R15" s="1"/>
+      <c r="S15" s="1"/>
+      <c r="T15" s="1"/>
+      <c r="U15" s="1"/>
+      <c r="V15" s="1"/>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
+      <c r="A16" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" s="1">
+        <v>5</v>
+      </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
+      <c r="H16" s="1">
+        <v>3</v>
+      </c>
       <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
+      <c r="J16" s="1">
+        <v>2</v>
+      </c>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
@@ -2951,8 +2971,12 @@
       <c r="V16" s="1"/>
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
+      <c r="A17" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" s="1">
+        <v>3</v>
+      </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
@@ -2960,7 +2984,9 @@
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
+      <c r="J17" s="1">
+        <v>2</v>
+      </c>
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
@@ -2975,8 +3001,12 @@
       <c r="V17" s="1"/>
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
+      <c r="A18" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" s="1">
+        <v>5</v>
+      </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
@@ -2984,9 +3014,15 @@
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
-      <c r="J18" s="1"/>
-      <c r="K18" s="1"/>
-      <c r="L18" s="1"/>
+      <c r="J18" s="1">
+        <v>3</v>
+      </c>
+      <c r="K18" s="1">
+        <v>1</v>
+      </c>
+      <c r="L18" s="1">
+        <v>2</v>
+      </c>
       <c r="M18" s="1"/>
       <c r="N18" s="1"/>
       <c r="O18" s="1"/>
@@ -2999,16 +3035,26 @@
       <c r="V18" s="1"/>
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
+      <c r="A19" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" s="1">
+        <v>3</v>
+      </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
+      <c r="H19" s="1">
+        <v>1</v>
+      </c>
+      <c r="I19" s="1">
+        <v>1</v>
+      </c>
+      <c r="J19" s="1">
+        <v>1</v>
+      </c>
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
       <c r="M19" s="1"/>
@@ -3023,23 +3069,35 @@
       <c r="V19" s="1"/>
     </row>
     <row r="20" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
+      <c r="A20" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20" s="1">
+        <v>5</v>
+      </c>
       <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
+      <c r="D20" s="1">
+        <v>1</v>
+      </c>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
+      <c r="G20" s="1">
+        <v>1</v>
+      </c>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
-      <c r="L20" s="1"/>
+      <c r="L20" s="1">
+        <v>1</v>
+      </c>
       <c r="M20" s="1"/>
       <c r="N20" s="1"/>
       <c r="O20" s="1"/>
       <c r="P20" s="1"/>
-      <c r="Q20" s="1"/>
+      <c r="Q20" s="1">
+        <v>1</v>
+      </c>
       <c r="R20" s="1"/>
       <c r="S20" s="1"/>
       <c r="T20" s="1"/>
@@ -3058,7 +3116,7 @@
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
-      <c r="L21" s="2"/>
+      <c r="L21" s="1"/>
       <c r="M21" s="1"/>
       <c r="N21" s="1"/>
       <c r="O21" s="1"/>
@@ -3069,6 +3127,235 @@
       <c r="T21" s="1"/>
       <c r="U21" s="1"/>
       <c r="V21" s="1"/>
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
+      <c r="L22" s="1"/>
+      <c r="M22" s="1"/>
+      <c r="N22" s="1"/>
+      <c r="O22" s="1"/>
+      <c r="P22" s="1"/>
+      <c r="Q22" s="1"/>
+      <c r="R22" s="1"/>
+      <c r="S22" s="1"/>
+      <c r="T22" s="1"/>
+      <c r="U22" s="1"/>
+      <c r="V22" s="1"/>
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+      <c r="L23" s="1"/>
+      <c r="M23" s="1"/>
+      <c r="N23" s="1"/>
+      <c r="O23" s="1"/>
+      <c r="P23" s="1"/>
+      <c r="Q23" s="1"/>
+      <c r="R23" s="1"/>
+      <c r="S23" s="1"/>
+      <c r="T23" s="1"/>
+      <c r="U23" s="1"/>
+      <c r="V23" s="1"/>
+    </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
+      <c r="L24" s="1"/>
+      <c r="M24" s="1"/>
+      <c r="N24" s="1"/>
+      <c r="O24" s="1"/>
+      <c r="P24" s="1"/>
+      <c r="Q24" s="1"/>
+      <c r="R24" s="1"/>
+      <c r="S24" s="1"/>
+      <c r="T24" s="1"/>
+      <c r="U24" s="1"/>
+      <c r="V24" s="1"/>
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B25" s="4">
+        <f>SUM(B2:B20)</f>
+        <v>86</v>
+      </c>
+      <c r="C25" s="4">
+        <f t="shared" ref="C25:V25" si="0">B25-SUM(C2:C20)</f>
+        <v>86</v>
+      </c>
+      <c r="D25" s="4">
+        <f t="shared" si="0"/>
+        <v>85</v>
+      </c>
+      <c r="E25" s="4">
+        <f t="shared" si="0"/>
+        <v>85</v>
+      </c>
+      <c r="F25" s="4">
+        <f t="shared" si="0"/>
+        <v>84</v>
+      </c>
+      <c r="G25" s="4">
+        <f t="shared" si="0"/>
+        <v>83</v>
+      </c>
+      <c r="H25" s="4">
+        <f t="shared" si="0"/>
+        <v>75</v>
+      </c>
+      <c r="I25" s="4">
+        <f t="shared" si="0"/>
+        <v>71</v>
+      </c>
+      <c r="J25" s="4">
+        <f t="shared" si="0"/>
+        <v>62</v>
+      </c>
+      <c r="K25" s="4">
+        <f t="shared" si="0"/>
+        <v>55</v>
+      </c>
+      <c r="L25" s="4">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="M25" s="4">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="N25" s="4">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="O25" s="4">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="P25" s="4">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="Q25" s="4">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="R25" s="4">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="S25" s="4">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="T25" s="4">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="U25" s="4">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="V25" s="4">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B26" s="6">
+        <v>86</v>
+      </c>
+      <c r="C26" s="6">
+        <v>81.7</v>
+      </c>
+      <c r="D26" s="6">
+        <v>77.400000000000006</v>
+      </c>
+      <c r="E26" s="6">
+        <v>73.099999999999994</v>
+      </c>
+      <c r="F26" s="6">
+        <v>68.8</v>
+      </c>
+      <c r="G26" s="6">
+        <v>64.5</v>
+      </c>
+      <c r="H26" s="6">
+        <v>60.2</v>
+      </c>
+      <c r="I26" s="6">
+        <v>55.9</v>
+      </c>
+      <c r="J26" s="6">
+        <v>51.6</v>
+      </c>
+      <c r="K26" s="6">
+        <v>47.3</v>
+      </c>
+      <c r="L26" s="6">
+        <v>43</v>
+      </c>
+      <c r="M26" s="6">
+        <v>38.700000000000003</v>
+      </c>
+      <c r="N26" s="6">
+        <v>34.4</v>
+      </c>
+      <c r="O26" s="6">
+        <v>30.1</v>
+      </c>
+      <c r="P26" s="6">
+        <v>25.8</v>
+      </c>
+      <c r="Q26" s="6">
+        <v>21.5</v>
+      </c>
+      <c r="R26" s="6">
+        <v>17.2</v>
+      </c>
+      <c r="S26" s="6">
+        <v>12.9</v>
+      </c>
+      <c r="T26" s="6">
+        <v>8.6000000000000902</v>
+      </c>
+      <c r="U26" s="6">
+        <v>4.3000000000001002</v>
+      </c>
+      <c r="V26" s="6">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
DOCS - burndown para reunião de scrum master
</commit_message>
<xml_diff>
--- a/DOCS/burndown_sprint.xlsx
+++ b/DOCS/burndown_sprint.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\FATEC\sem2\API-2\DOCS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B431E395-FF05-42FC-B301-B77283407DAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9A09281-7734-46A6-8CD2-F24617BBCCCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Burndown Chart" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t>Total de horas</t>
   </si>
@@ -163,6 +163,12 @@
   </si>
   <si>
     <t>US-1.2 (caio, back)</t>
+  </si>
+  <si>
+    <t>US-1.9 ( caio, back)</t>
+  </si>
+  <si>
+    <t>US-3.4 (daniel, full-stack)</t>
   </si>
 </sst>
 </file>
@@ -916,67 +922,67 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>86</c:v>
+                  <c:v>99</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>86</c:v>
+                  <c:v>98</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>85</c:v>
+                  <c:v>97</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>85</c:v>
+                  <c:v>97</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>84</c:v>
+                  <c:v>96</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>87</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>83</c:v>
                 </c:pt>
-                <c:pt idx="6">
-                  <c:v>75</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>71</c:v>
-                </c:pt>
                 <c:pt idx="8">
-                  <c:v>62</c:v>
+                  <c:v>74</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>55</c:v>
+                  <c:v>67</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>45</c:v>
+                  <c:v>57</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>42</c:v>
+                  <c:v>53</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>39</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>39</c:v>
+                  <c:v>47</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>37</c:v>
+                  <c:v>44</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>36</c:v>
+                  <c:v>34.5</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>36</c:v>
+                  <c:v>25.5</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>36</c:v>
+                  <c:v>25.5</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>36</c:v>
+                  <c:v>25.5</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>36</c:v>
+                  <c:v>25.5</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>36</c:v>
+                  <c:v>25.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1090,64 +1096,64 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>86</c:v>
+                  <c:v>99</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>81.7</c:v>
+                  <c:v>94.05</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>77.400000000000006</c:v>
+                  <c:v>89.1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>73.099999999999994</c:v>
+                  <c:v>84.15</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>68.8</c:v>
+                  <c:v>79.2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>64.5</c:v>
+                  <c:v>74.25</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>60.2</c:v>
+                  <c:v>69.3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>55.9</c:v>
+                  <c:v>64.349999999999994</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>51.6</c:v>
+                  <c:v>59.4</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>47.3</c:v>
+                  <c:v>54.45</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43</c:v>
+                  <c:v>49.5</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>38.700000000000003</c:v>
+                  <c:v>44.55</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>34.4</c:v>
+                  <c:v>39.6</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>30.1</c:v>
+                  <c:v>34.65</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>25.8</c:v>
+                  <c:v>29.7</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>21.5</c:v>
+                  <c:v>24.75</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>17.2</c:v>
+                  <c:v>19.8</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>12.9</c:v>
+                  <c:v>14.85</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>8.6000000000000902</c:v>
+                  <c:v>9.8999999999999098</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>4.3000000000001002</c:v>
+                  <c:v>4.9499999999998998</c:v>
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>0</c:v>
@@ -1559,67 +1565,67 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>86</c:v>
+                  <c:v>99</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>86</c:v>
+                  <c:v>98</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>85</c:v>
+                  <c:v>97</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>85</c:v>
+                  <c:v>97</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>84</c:v>
+                  <c:v>96</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>87</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>83</c:v>
                 </c:pt>
-                <c:pt idx="6">
-                  <c:v>75</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>71</c:v>
-                </c:pt>
                 <c:pt idx="8">
-                  <c:v>62</c:v>
+                  <c:v>74</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>55</c:v>
+                  <c:v>67</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>45</c:v>
+                  <c:v>57</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>42</c:v>
+                  <c:v>53</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>39</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>39</c:v>
+                  <c:v>47</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>37</c:v>
+                  <c:v>44</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>36</c:v>
+                  <c:v>34.5</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>36</c:v>
+                  <c:v>25.5</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>36</c:v>
+                  <c:v>25.5</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>36</c:v>
+                  <c:v>25.5</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>36</c:v>
+                  <c:v>25.5</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>36</c:v>
+                  <c:v>25.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1733,64 +1739,64 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>86</c:v>
+                  <c:v>99</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>81.7</c:v>
+                  <c:v>94.05</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>77.400000000000006</c:v>
+                  <c:v>89.1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>73.099999999999994</c:v>
+                  <c:v>84.15</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>68.8</c:v>
+                  <c:v>79.2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>64.5</c:v>
+                  <c:v>74.25</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>60.2</c:v>
+                  <c:v>69.3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>55.9</c:v>
+                  <c:v>64.349999999999994</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>51.6</c:v>
+                  <c:v>59.4</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>47.3</c:v>
+                  <c:v>54.45</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43</c:v>
+                  <c:v>49.5</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>38.700000000000003</c:v>
+                  <c:v>44.55</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>34.4</c:v>
+                  <c:v>39.6</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>30.1</c:v>
+                  <c:v>34.65</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>25.8</c:v>
+                  <c:v>29.7</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>21.5</c:v>
+                  <c:v>24.75</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>17.2</c:v>
+                  <c:v>19.8</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>12.9</c:v>
+                  <c:v>14.85</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>8.6000000000000902</c:v>
+                  <c:v>9.8999999999999098</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>4.3000000000001002</c:v>
+                  <c:v>4.9499999999998998</c:v>
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>0</c:v>
@@ -2427,13 +2433,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q21" sqref="Q21"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="V36" sqref="V36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="11" width="9.85546875" bestFit="1" customWidth="1"/>
@@ -2527,7 +2533,9 @@
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
+      <c r="M2" s="1">
+        <v>1</v>
+      </c>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
@@ -2561,7 +2569,9 @@
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
-      <c r="Q3" s="1"/>
+      <c r="Q3" s="1">
+        <v>1</v>
+      </c>
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
       <c r="T3" s="1"/>
@@ -2573,7 +2583,7 @@
         <v>32</v>
       </c>
       <c r="B4" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -2588,13 +2598,17 @@
       </c>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
-      <c r="N4" s="1"/>
+      <c r="N4" s="1">
+        <v>1</v>
+      </c>
       <c r="O4" s="1"/>
       <c r="P4" s="1">
         <v>1</v>
       </c>
       <c r="Q4" s="1"/>
-      <c r="R4" s="1"/>
+      <c r="R4" s="1">
+        <v>1</v>
+      </c>
       <c r="S4" s="1"/>
       <c r="T4" s="1"/>
       <c r="U4" s="1"/>
@@ -2622,7 +2636,9 @@
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
       <c r="Q5" s="1"/>
-      <c r="R5" s="1"/>
+      <c r="R5" s="1">
+        <v>1</v>
+      </c>
       <c r="S5" s="1"/>
       <c r="T5" s="1"/>
       <c r="U5" s="1"/>
@@ -2722,10 +2738,10 @@
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B9" s="1">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -2733,31 +2749,31 @@
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
-      <c r="I9" s="1">
-        <v>1</v>
-      </c>
+      <c r="I9" s="1"/>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
-      <c r="M9" s="1">
-        <v>2</v>
-      </c>
+      <c r="M9" s="1"/>
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
-      <c r="Q9" s="1"/>
-      <c r="R9" s="1"/>
+      <c r="Q9" s="1">
+        <v>2</v>
+      </c>
+      <c r="R9" s="1">
+        <v>2</v>
+      </c>
       <c r="S9" s="1"/>
       <c r="T9" s="1"/>
       <c r="U9" s="1"/>
       <c r="V9" s="1"/>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>38</v>
+      <c r="A10" s="1" t="s">
+        <v>39</v>
       </c>
       <c r="B10" s="1">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -2766,18 +2782,20 @@
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
-      <c r="L10" s="1">
-        <v>3</v>
-      </c>
-      <c r="M10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1">
+        <v>2</v>
+      </c>
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
-      <c r="Q10" s="1"/>
+      <c r="Q10" s="1">
+        <v>2.5</v>
+      </c>
       <c r="R10" s="1"/>
       <c r="S10" s="1"/>
       <c r="T10" s="1"/>
@@ -2785,11 +2803,11 @@
       <c r="V10" s="1"/>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>34</v>
+      <c r="A11" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="B11" s="1">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
@@ -2797,11 +2815,13 @@
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
+      <c r="I11" s="1">
+        <v>2</v>
+      </c>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
       <c r="L11" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="M11" s="1"/>
       <c r="N11" s="1"/>
@@ -2815,8 +2835,8 @@
       <c r="V11" s="1"/>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>35</v>
+      <c r="A12" s="1" t="s">
+        <v>34</v>
       </c>
       <c r="B12" s="1">
         <v>8</v>
@@ -2830,7 +2850,9 @@
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
-      <c r="L12" s="1"/>
+      <c r="L12" s="1">
+        <v>1</v>
+      </c>
       <c r="M12" s="1"/>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
@@ -2843,8 +2865,8 @@
       <c r="V12" s="1"/>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>36</v>
+      <c r="A13" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="B13" s="1">
         <v>8</v>
@@ -2856,25 +2878,29 @@
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
-      <c r="J13" s="1">
-        <v>1</v>
-      </c>
+      <c r="J13" s="1"/>
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
-      <c r="P13" s="1"/>
-      <c r="Q13" s="1"/>
-      <c r="R13" s="1"/>
+      <c r="P13" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q13" s="1">
+        <v>1</v>
+      </c>
+      <c r="R13" s="1">
+        <v>2</v>
+      </c>
       <c r="S13" s="1"/>
       <c r="T13" s="1"/>
       <c r="U13" s="1"/>
       <c r="V13" s="1"/>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>37</v>
+      <c r="A14" s="1" t="s">
+        <v>36</v>
       </c>
       <c r="B14" s="1">
         <v>8</v>
@@ -2886,19 +2912,15 @@
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
+      <c r="J14" s="1">
+        <v>1</v>
+      </c>
       <c r="K14" s="1"/>
-      <c r="L14" s="1">
-        <v>1</v>
-      </c>
-      <c r="M14" s="1">
-        <v>1</v>
-      </c>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
-      <c r="P14" s="1">
-        <v>1</v>
-      </c>
+      <c r="P14" s="1"/>
       <c r="Q14" s="1"/>
       <c r="R14" s="1"/>
       <c r="S14" s="1"/>
@@ -2908,29 +2930,31 @@
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="B15" s="1">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
-      <c r="F15" s="1">
-        <v>1</v>
-      </c>
+      <c r="F15" s="1"/>
       <c r="G15" s="1"/>
-      <c r="H15" s="1">
-        <v>2</v>
-      </c>
+      <c r="H15" s="1"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
-      <c r="L15" s="1"/>
-      <c r="M15" s="1"/>
+      <c r="L15" s="1">
+        <v>1</v>
+      </c>
+      <c r="M15" s="1">
+        <v>1</v>
+      </c>
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
-      <c r="P15" s="1"/>
+      <c r="P15" s="1">
+        <v>1</v>
+      </c>
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
       <c r="S15" s="1"/>
@@ -2939,44 +2963,40 @@
       <c r="V15" s="1"/>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>24</v>
+      <c r="A16" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="B16" s="1">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
-      <c r="H16" s="1">
-        <v>3</v>
-      </c>
+      <c r="H16" s="1"/>
       <c r="I16" s="1"/>
-      <c r="J16" s="1">
-        <v>2</v>
-      </c>
+      <c r="J16" s="1"/>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
       <c r="N16" s="1"/>
       <c r="O16" s="1"/>
       <c r="P16" s="1"/>
-      <c r="Q16" s="1"/>
-      <c r="R16" s="1"/>
+      <c r="Q16" s="1">
+        <v>2</v>
+      </c>
+      <c r="R16" s="1">
+        <v>3</v>
+      </c>
       <c r="S16" s="1"/>
       <c r="T16" s="1"/>
       <c r="U16" s="1"/>
       <c r="V16" s="1"/>
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B17" s="1">
-        <v>3</v>
-      </c>
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
@@ -2984,9 +3004,7 @@
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
-      <c r="J17" s="1">
-        <v>2</v>
-      </c>
+      <c r="J17" s="1"/>
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
@@ -3001,12 +3019,8 @@
       <c r="V17" s="1"/>
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B18" s="1">
-        <v>5</v>
-      </c>
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
@@ -3014,15 +3028,9 @@
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
-      <c r="J18" s="1">
-        <v>3</v>
-      </c>
-      <c r="K18" s="1">
-        <v>1</v>
-      </c>
-      <c r="L18" s="1">
-        <v>2</v>
-      </c>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
       <c r="M18" s="1"/>
       <c r="N18" s="1"/>
       <c r="O18" s="1"/>
@@ -3036,7 +3044,7 @@
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B19" s="1">
         <v>3</v>
@@ -3044,17 +3052,15 @@
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
+      <c r="F19" s="1">
+        <v>1</v>
+      </c>
       <c r="G19" s="1"/>
       <c r="H19" s="1">
-        <v>1</v>
-      </c>
-      <c r="I19" s="1">
-        <v>1</v>
-      </c>
-      <c r="J19" s="1">
-        <v>1</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
       <c r="M19" s="1"/>
@@ -3069,35 +3075,31 @@
       <c r="V19" s="1"/>
     </row>
     <row r="20" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>28</v>
+      <c r="A20" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="B20" s="1">
         <v>5</v>
       </c>
       <c r="C20" s="1"/>
-      <c r="D20" s="1">
-        <v>1</v>
-      </c>
+      <c r="D20" s="1"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
-      <c r="G20" s="1">
-        <v>1</v>
-      </c>
-      <c r="H20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1">
+        <v>3</v>
+      </c>
       <c r="I20" s="1"/>
-      <c r="J20" s="1"/>
+      <c r="J20" s="1">
+        <v>2</v>
+      </c>
       <c r="K20" s="1"/>
-      <c r="L20" s="1">
-        <v>1</v>
-      </c>
+      <c r="L20" s="1"/>
       <c r="M20" s="1"/>
       <c r="N20" s="1"/>
       <c r="O20" s="1"/>
       <c r="P20" s="1"/>
-      <c r="Q20" s="1">
-        <v>1</v>
-      </c>
+      <c r="Q20" s="1"/>
       <c r="R20" s="1"/>
       <c r="S20" s="1"/>
       <c r="T20" s="1"/>
@@ -3105,8 +3107,12 @@
       <c r="V20" s="1"/>
     </row>
     <row r="21" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
+      <c r="A21" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21" s="1">
+        <v>3</v>
+      </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
@@ -3114,11 +3120,15 @@
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
-      <c r="J21" s="1"/>
+      <c r="J21" s="1">
+        <v>2</v>
+      </c>
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
       <c r="M21" s="1"/>
-      <c r="N21" s="1"/>
+      <c r="N21" s="1">
+        <v>1</v>
+      </c>
       <c r="O21" s="1"/>
       <c r="P21" s="1"/>
       <c r="Q21" s="1"/>
@@ -3129,8 +3139,12 @@
       <c r="V21" s="1"/>
     </row>
     <row r="22" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
+      <c r="A22" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B22" s="1">
+        <v>5</v>
+      </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
@@ -3138,9 +3152,15 @@
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
-      <c r="J22" s="1"/>
-      <c r="K22" s="1"/>
-      <c r="L22" s="1"/>
+      <c r="J22" s="1">
+        <v>3</v>
+      </c>
+      <c r="K22" s="1">
+        <v>1</v>
+      </c>
+      <c r="L22" s="1">
+        <v>2</v>
+      </c>
       <c r="M22" s="1"/>
       <c r="N22" s="1"/>
       <c r="O22" s="1"/>
@@ -3153,16 +3173,26 @@
       <c r="V22" s="1"/>
     </row>
     <row r="23" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
+      <c r="A23" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B23" s="1">
+        <v>3</v>
+      </c>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
-      <c r="J23" s="1"/>
+      <c r="H23" s="1">
+        <v>1</v>
+      </c>
+      <c r="I23" s="1">
+        <v>1</v>
+      </c>
+      <c r="J23" s="1">
+        <v>1</v>
+      </c>
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
       <c r="M23" s="1"/>
@@ -3177,23 +3207,39 @@
       <c r="V23" s="1"/>
     </row>
     <row r="24" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
+      <c r="A24" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B24" s="1">
+        <v>5</v>
+      </c>
+      <c r="C24" s="1">
+        <v>1</v>
+      </c>
+      <c r="D24" s="1">
+        <v>1</v>
+      </c>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
+      <c r="G24" s="1">
+        <v>1</v>
+      </c>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
-      <c r="L24" s="1"/>
+      <c r="L24" s="1">
+        <v>1</v>
+      </c>
       <c r="M24" s="1"/>
       <c r="N24" s="1"/>
-      <c r="O24" s="1"/>
+      <c r="O24" s="1">
+        <v>1</v>
+      </c>
       <c r="P24" s="1"/>
-      <c r="Q24" s="1"/>
+      <c r="Q24" s="1">
+        <v>1</v>
+      </c>
       <c r="R24" s="1"/>
       <c r="S24" s="1"/>
       <c r="T24" s="1"/>
@@ -3205,88 +3251,88 @@
         <v>21</v>
       </c>
       <c r="B25" s="4">
-        <f>SUM(B2:B20)</f>
-        <v>86</v>
+        <f>SUM(B2:B24)</f>
+        <v>99</v>
       </c>
       <c r="C25" s="4">
-        <f t="shared" ref="C25:V25" si="0">B25-SUM(C2:C20)</f>
-        <v>86</v>
+        <f>B25-SUM(C2:C24)</f>
+        <v>98</v>
       </c>
       <c r="D25" s="4">
-        <f t="shared" si="0"/>
-        <v>85</v>
+        <f>C25-SUM(D2:D24)</f>
+        <v>97</v>
       </c>
       <c r="E25" s="4">
-        <f t="shared" si="0"/>
-        <v>85</v>
+        <f>D25-SUM(E2:E24)</f>
+        <v>97</v>
       </c>
       <c r="F25" s="4">
-        <f t="shared" si="0"/>
-        <v>84</v>
+        <f>E25-SUM(F2:F24)</f>
+        <v>96</v>
       </c>
       <c r="G25" s="4">
-        <f t="shared" si="0"/>
+        <f>F25-SUM(G2:G24)</f>
+        <v>95</v>
+      </c>
+      <c r="H25" s="4">
+        <f>G25-SUM(H2:H24)</f>
+        <v>87</v>
+      </c>
+      <c r="I25" s="4">
+        <f>H25-SUM(I2:I24)</f>
         <v>83</v>
       </c>
-      <c r="H25" s="4">
-        <f t="shared" si="0"/>
-        <v>75</v>
-      </c>
-      <c r="I25" s="4">
-        <f t="shared" si="0"/>
-        <v>71</v>
-      </c>
       <c r="J25" s="4">
-        <f t="shared" si="0"/>
-        <v>62</v>
+        <f>I25-SUM(J2:J24)</f>
+        <v>74</v>
       </c>
       <c r="K25" s="4">
-        <f t="shared" si="0"/>
-        <v>55</v>
+        <f>J25-SUM(K2:K24)</f>
+        <v>67</v>
       </c>
       <c r="L25" s="4">
-        <f t="shared" si="0"/>
-        <v>45</v>
+        <f>K25-SUM(L2:L24)</f>
+        <v>57</v>
       </c>
       <c r="M25" s="4">
-        <f t="shared" si="0"/>
-        <v>42</v>
+        <f>L25-SUM(M2:M24)</f>
+        <v>53</v>
       </c>
       <c r="N25" s="4">
-        <f t="shared" si="0"/>
-        <v>39</v>
+        <f>M25-SUM(N2:N24)</f>
+        <v>48</v>
       </c>
       <c r="O25" s="4">
-        <f t="shared" si="0"/>
-        <v>39</v>
+        <f>N25-SUM(O2:O24)</f>
+        <v>47</v>
       </c>
       <c r="P25" s="4">
-        <f t="shared" si="0"/>
-        <v>37</v>
+        <f>O25-SUM(P2:P24)</f>
+        <v>44</v>
       </c>
       <c r="Q25" s="4">
-        <f t="shared" si="0"/>
-        <v>36</v>
+        <f>P25-SUM(Q2:Q24)</f>
+        <v>34.5</v>
       </c>
       <c r="R25" s="4">
-        <f t="shared" si="0"/>
-        <v>36</v>
+        <f>Q25-SUM(R2:R24)</f>
+        <v>25.5</v>
       </c>
       <c r="S25" s="4">
-        <f t="shared" si="0"/>
-        <v>36</v>
+        <f>R25-SUM(S2:S24)</f>
+        <v>25.5</v>
       </c>
       <c r="T25" s="4">
-        <f t="shared" si="0"/>
-        <v>36</v>
+        <f>S25-SUM(T2:T24)</f>
+        <v>25.5</v>
       </c>
       <c r="U25" s="4">
-        <f t="shared" si="0"/>
-        <v>36</v>
+        <f>T25-SUM(U2:U24)</f>
+        <v>25.5</v>
       </c>
       <c r="V25" s="4">
-        <f t="shared" si="0"/>
-        <v>36</v>
+        <f>U25-SUM(V2:V24)</f>
+        <v>25.5</v>
       </c>
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.25">
@@ -3294,64 +3340,64 @@
         <v>22</v>
       </c>
       <c r="B26" s="6">
-        <v>86</v>
+        <v>99</v>
       </c>
       <c r="C26" s="6">
-        <v>81.7</v>
+        <v>94.05</v>
       </c>
       <c r="D26" s="6">
-        <v>77.400000000000006</v>
+        <v>89.1</v>
       </c>
       <c r="E26" s="6">
-        <v>73.099999999999994</v>
+        <v>84.15</v>
       </c>
       <c r="F26" s="6">
-        <v>68.8</v>
+        <v>79.2</v>
       </c>
       <c r="G26" s="6">
-        <v>64.5</v>
+        <v>74.25</v>
       </c>
       <c r="H26" s="6">
-        <v>60.2</v>
+        <v>69.3</v>
       </c>
       <c r="I26" s="6">
-        <v>55.9</v>
+        <v>64.349999999999994</v>
       </c>
       <c r="J26" s="6">
-        <v>51.6</v>
+        <v>59.4</v>
       </c>
       <c r="K26" s="6">
-        <v>47.3</v>
+        <v>54.45</v>
       </c>
       <c r="L26" s="6">
-        <v>43</v>
+        <v>49.5</v>
       </c>
       <c r="M26" s="6">
-        <v>38.700000000000003</v>
+        <v>44.55</v>
       </c>
       <c r="N26" s="6">
-        <v>34.4</v>
+        <v>39.6</v>
       </c>
       <c r="O26" s="6">
-        <v>30.1</v>
+        <v>34.65</v>
       </c>
       <c r="P26" s="6">
-        <v>25.8</v>
+        <v>29.7</v>
       </c>
       <c r="Q26" s="6">
-        <v>21.5</v>
+        <v>24.75</v>
       </c>
       <c r="R26" s="6">
-        <v>17.2</v>
+        <v>19.8</v>
       </c>
       <c r="S26" s="6">
-        <v>12.9</v>
+        <v>14.85</v>
       </c>
       <c r="T26" s="6">
-        <v>8.6000000000000902</v>
+        <v>9.8999999999999098</v>
       </c>
       <c r="U26" s="6">
-        <v>4.3000000000001002</v>
+        <v>4.9499999999998998</v>
       </c>
       <c r="V26" s="6">
         <v>0</v>
@@ -3371,8 +3417,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7AEF5D5-9845-4510-B31C-B45C1A0563CA}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="S33" sqref="S33"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="N34" sqref="N34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
DELETE - remocao do colaborador dentro do sistema
</commit_message>
<xml_diff>
--- a/DOCS/burndown_sprint.xlsx
+++ b/DOCS/burndown_sprint.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\FATEC\sem2\API-2\DOCS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9A09281-7734-46A6-8CD2-F24617BBCCCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F355B14-FEB2-4CBB-9201-1DE13C55FE27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Burndown Chart" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>Total de horas</t>
   </si>
@@ -138,15 +138,9 @@
     <t>US-1.1 (Banco)</t>
   </si>
   <si>
-    <t>US-1.4 (gabriel, front)</t>
-  </si>
-  <si>
     <t>US-1.5 (giovanni, front)</t>
   </si>
   <si>
-    <t>US-2.3 (giovanni, front)</t>
-  </si>
-  <si>
     <t>US-3.2 (gabriel, front)</t>
   </si>
   <si>
@@ -169,6 +163,15 @@
   </si>
   <si>
     <t>US-3.4 (daniel, full-stack)</t>
+  </si>
+  <si>
+    <t>US-2.3 (monteiro, front)</t>
+  </si>
+  <si>
+    <t>US-2.4 (monteiro, back)</t>
+  </si>
+  <si>
+    <t>US-1.4 (caio, front)</t>
   </si>
 </sst>
 </file>
@@ -922,67 +925,67 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
+                  <c:v>102</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>101</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>99</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="5">
                   <c:v>98</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>97</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>97</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>96</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>95</c:v>
-                </c:pt>
                 <c:pt idx="6">
-                  <c:v>87</c:v>
+                  <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>83</c:v>
+                  <c:v>86</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>74</c:v>
+                  <c:v>77</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>67</c:v>
+                  <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>57</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>53</c:v>
+                  <c:v>56</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>48</c:v>
+                  <c:v>51</c:v>
                 </c:pt>
                 <c:pt idx="13">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="14">
                   <c:v>47</c:v>
                 </c:pt>
-                <c:pt idx="14">
-                  <c:v>44</c:v>
-                </c:pt>
                 <c:pt idx="15">
-                  <c:v>34.5</c:v>
+                  <c:v>37.5</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>25.5</c:v>
+                  <c:v>23.5</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>25.5</c:v>
+                  <c:v>13.5</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>25.5</c:v>
+                  <c:v>7.5</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>25.5</c:v>
+                  <c:v>1.5</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>25.5</c:v>
+                  <c:v>-1.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1096,64 +1099,64 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>99</c:v>
+                  <c:v>102</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>94.05</c:v>
+                  <c:v>96.9</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>89.1</c:v>
+                  <c:v>91.8</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>84.15</c:v>
+                  <c:v>86.7</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>79.2</c:v>
+                  <c:v>81.599999999999994</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>74.25</c:v>
+                  <c:v>76.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>69.3</c:v>
+                  <c:v>71.400000000000006</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>64.349999999999994</c:v>
+                  <c:v>66.3</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>59.4</c:v>
+                  <c:v>61.2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>54.45</c:v>
+                  <c:v>56.100000000000101</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>49.5</c:v>
+                  <c:v>51.000000000000099</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44.55</c:v>
+                  <c:v>45.900000000000098</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>39.6</c:v>
+                  <c:v>40.800000000000097</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>34.65</c:v>
+                  <c:v>35.700000000000102</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>29.7</c:v>
+                  <c:v>30.600000000000101</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>24.75</c:v>
+                  <c:v>25.500000000000099</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>19.8</c:v>
+                  <c:v>20.400000000000102</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>14.85</c:v>
+                  <c:v>15.3000000000001</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>9.8999999999999098</c:v>
+                  <c:v>10.200000000000101</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>4.9499999999998998</c:v>
+                  <c:v>5.1000000000000902</c:v>
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>0</c:v>
@@ -1565,67 +1568,67 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
+                  <c:v>102</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>101</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>99</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="5">
                   <c:v>98</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>97</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>97</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>96</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>95</c:v>
-                </c:pt>
                 <c:pt idx="6">
-                  <c:v>87</c:v>
+                  <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>83</c:v>
+                  <c:v>86</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>74</c:v>
+                  <c:v>77</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>67</c:v>
+                  <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>57</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>53</c:v>
+                  <c:v>56</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>48</c:v>
+                  <c:v>51</c:v>
                 </c:pt>
                 <c:pt idx="13">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="14">
                   <c:v>47</c:v>
                 </c:pt>
-                <c:pt idx="14">
-                  <c:v>44</c:v>
-                </c:pt>
                 <c:pt idx="15">
-                  <c:v>34.5</c:v>
+                  <c:v>37.5</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>25.5</c:v>
+                  <c:v>23.5</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>25.5</c:v>
+                  <c:v>13.5</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>25.5</c:v>
+                  <c:v>7.5</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>25.5</c:v>
+                  <c:v>1.5</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>25.5</c:v>
+                  <c:v>-1.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1739,64 +1742,64 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>99</c:v>
+                  <c:v>102</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>94.05</c:v>
+                  <c:v>96.9</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>89.1</c:v>
+                  <c:v>91.8</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>84.15</c:v>
+                  <c:v>86.7</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>79.2</c:v>
+                  <c:v>81.599999999999994</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>74.25</c:v>
+                  <c:v>76.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>69.3</c:v>
+                  <c:v>71.400000000000006</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>64.349999999999994</c:v>
+                  <c:v>66.3</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>59.4</c:v>
+                  <c:v>61.2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>54.45</c:v>
+                  <c:v>56.100000000000101</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>49.5</c:v>
+                  <c:v>51.000000000000099</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44.55</c:v>
+                  <c:v>45.900000000000098</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>39.6</c:v>
+                  <c:v>40.800000000000097</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>34.65</c:v>
+                  <c:v>35.700000000000102</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>29.7</c:v>
+                  <c:v>30.600000000000101</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>24.75</c:v>
+                  <c:v>25.500000000000099</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>19.8</c:v>
+                  <c:v>20.400000000000102</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>14.85</c:v>
+                  <c:v>15.3000000000001</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>9.8999999999999098</c:v>
+                  <c:v>10.200000000000101</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>4.9499999999998998</c:v>
+                  <c:v>5.1000000000000902</c:v>
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>0</c:v>
@@ -2433,8 +2436,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V26"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="V36" sqref="V36"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AE25" sqref="AE25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2607,9 +2610,11 @@
       </c>
       <c r="Q4" s="1"/>
       <c r="R4" s="1">
-        <v>1</v>
-      </c>
-      <c r="S4" s="1"/>
+        <v>2</v>
+      </c>
+      <c r="S4" s="1">
+        <v>1</v>
+      </c>
       <c r="T4" s="1"/>
       <c r="U4" s="1"/>
       <c r="V4" s="1"/>
@@ -2619,7 +2624,7 @@
         <v>31</v>
       </c>
       <c r="B5" s="1">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -2639,14 +2644,22 @@
       <c r="R5" s="1">
         <v>1</v>
       </c>
-      <c r="S5" s="1"/>
-      <c r="T5" s="1"/>
-      <c r="U5" s="1"/>
-      <c r="V5" s="1"/>
+      <c r="S5" s="1">
+        <v>2</v>
+      </c>
+      <c r="T5" s="1">
+        <v>1</v>
+      </c>
+      <c r="U5" s="1">
+        <v>2</v>
+      </c>
+      <c r="V5" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B6" s="1">
         <v>1</v>
@@ -2676,7 +2689,7 @@
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B7" s="1">
         <v>5</v>
@@ -2708,7 +2721,7 @@
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B8" s="1">
         <v>3</v>
@@ -2738,7 +2751,7 @@
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B9" s="1">
         <v>3</v>
@@ -2770,7 +2783,7 @@
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B10" s="1">
         <v>8</v>
@@ -2796,15 +2809,19 @@
       <c r="Q10" s="1">
         <v>2.5</v>
       </c>
-      <c r="R10" s="1"/>
-      <c r="S10" s="1"/>
+      <c r="R10" s="1">
+        <v>2</v>
+      </c>
+      <c r="S10" s="1">
+        <v>2</v>
+      </c>
       <c r="T10" s="1"/>
       <c r="U10" s="1"/>
       <c r="V10" s="1"/>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B11" s="1">
         <v>5</v>
@@ -2828,15 +2845,17 @@
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
       <c r="Q11" s="1"/>
-      <c r="R11" s="1"/>
+      <c r="R11" s="1">
+        <v>1</v>
+      </c>
       <c r="S11" s="1"/>
       <c r="T11" s="1"/>
       <c r="U11" s="1"/>
       <c r="V11" s="1"/>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>34</v>
+      <c r="A12" s="2" t="s">
+        <v>45</v>
       </c>
       <c r="B12" s="1">
         <v>8</v>
@@ -2858,15 +2877,19 @@
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
       <c r="Q12" s="1"/>
-      <c r="R12" s="1"/>
-      <c r="S12" s="1"/>
+      <c r="R12" s="1">
+        <v>1</v>
+      </c>
+      <c r="S12" s="1">
+        <v>1</v>
+      </c>
       <c r="T12" s="1"/>
       <c r="U12" s="1"/>
       <c r="V12" s="1"/>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B13" s="1">
         <v>8</v>
@@ -2899,11 +2922,11 @@
       <c r="V13" s="1"/>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>36</v>
+      <c r="A14" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="B14" s="1">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -2923,17 +2946,21 @@
       <c r="P14" s="1"/>
       <c r="Q14" s="1"/>
       <c r="R14" s="1"/>
-      <c r="S14" s="1"/>
-      <c r="T14" s="1"/>
+      <c r="S14" s="1">
+        <v>1</v>
+      </c>
+      <c r="T14" s="1">
+        <v>2</v>
+      </c>
       <c r="U14" s="1"/>
       <c r="V14" s="1"/>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>37</v>
+      <c r="A15" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="B15" s="1">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
@@ -2944,27 +2971,25 @@
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
-      <c r="L15" s="1">
-        <v>1</v>
-      </c>
-      <c r="M15" s="1">
-        <v>1</v>
-      </c>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
-      <c r="P15" s="1">
-        <v>1</v>
-      </c>
+      <c r="P15" s="1"/>
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
-      <c r="S15" s="1"/>
-      <c r="T15" s="1"/>
+      <c r="S15" s="1">
+        <v>2</v>
+      </c>
+      <c r="T15" s="1">
+        <v>2</v>
+      </c>
       <c r="U15" s="1"/>
       <c r="V15" s="1"/>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>44</v>
+      <c r="A16" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="B16" s="1">
         <v>8</v>
@@ -2978,25 +3003,35 @@
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
-      <c r="L16" s="1"/>
-      <c r="M16" s="1"/>
+      <c r="L16" s="1">
+        <v>1</v>
+      </c>
+      <c r="M16" s="1">
+        <v>1</v>
+      </c>
       <c r="N16" s="1"/>
       <c r="O16" s="1"/>
-      <c r="P16" s="1"/>
-      <c r="Q16" s="1">
-        <v>2</v>
-      </c>
-      <c r="R16" s="1">
-        <v>3</v>
-      </c>
+      <c r="P16" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q16" s="1"/>
+      <c r="R16" s="1"/>
       <c r="S16" s="1"/>
       <c r="T16" s="1"/>
-      <c r="U16" s="1"/>
-      <c r="V16" s="1"/>
+      <c r="U16" s="1">
+        <v>2</v>
+      </c>
+      <c r="V16" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
+      <c r="A17" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17" s="1">
+        <v>8</v>
+      </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
@@ -3011,12 +3046,22 @@
       <c r="N17" s="1"/>
       <c r="O17" s="1"/>
       <c r="P17" s="1"/>
-      <c r="Q17" s="1"/>
-      <c r="R17" s="1"/>
+      <c r="Q17" s="1">
+        <v>2</v>
+      </c>
+      <c r="R17" s="1">
+        <v>3</v>
+      </c>
       <c r="S17" s="1"/>
-      <c r="T17" s="1"/>
-      <c r="U17" s="1"/>
-      <c r="V17" s="1"/>
+      <c r="T17" s="1">
+        <v>1</v>
+      </c>
+      <c r="U17" s="1">
+        <v>2</v>
+      </c>
+      <c r="V17" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
@@ -3241,7 +3286,9 @@
         <v>1</v>
       </c>
       <c r="R24" s="1"/>
-      <c r="S24" s="1"/>
+      <c r="S24" s="1">
+        <v>1</v>
+      </c>
       <c r="T24" s="1"/>
       <c r="U24" s="1"/>
       <c r="V24" s="1"/>
@@ -3252,87 +3299,87 @@
       </c>
       <c r="B25" s="4">
         <f>SUM(B2:B24)</f>
+        <v>102</v>
+      </c>
+      <c r="C25" s="4">
+        <f t="shared" ref="C25:V25" si="0">B25-SUM(C2:C24)</f>
+        <v>101</v>
+      </c>
+      <c r="D25" s="4">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="E25" s="4">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="F25" s="4">
+        <f t="shared" si="0"/>
         <v>99</v>
       </c>
-      <c r="C25" s="4">
-        <f>B25-SUM(C2:C24)</f>
+      <c r="G25" s="4">
+        <f t="shared" si="0"/>
         <v>98</v>
       </c>
-      <c r="D25" s="4">
-        <f>C25-SUM(D2:D24)</f>
-        <v>97</v>
-      </c>
-      <c r="E25" s="4">
-        <f>D25-SUM(E2:E24)</f>
-        <v>97</v>
-      </c>
-      <c r="F25" s="4">
-        <f>E25-SUM(F2:F24)</f>
-        <v>96</v>
-      </c>
-      <c r="G25" s="4">
-        <f>F25-SUM(G2:G24)</f>
-        <v>95</v>
-      </c>
       <c r="H25" s="4">
-        <f>G25-SUM(H2:H24)</f>
-        <v>87</v>
+        <f t="shared" si="0"/>
+        <v>90</v>
       </c>
       <c r="I25" s="4">
-        <f>H25-SUM(I2:I24)</f>
-        <v>83</v>
+        <f t="shared" si="0"/>
+        <v>86</v>
       </c>
       <c r="J25" s="4">
-        <f>I25-SUM(J2:J24)</f>
-        <v>74</v>
+        <f t="shared" si="0"/>
+        <v>77</v>
       </c>
       <c r="K25" s="4">
-        <f>J25-SUM(K2:K24)</f>
-        <v>67</v>
+        <f t="shared" si="0"/>
+        <v>70</v>
       </c>
       <c r="L25" s="4">
-        <f>K25-SUM(L2:L24)</f>
-        <v>57</v>
+        <f t="shared" si="0"/>
+        <v>60</v>
       </c>
       <c r="M25" s="4">
-        <f>L25-SUM(M2:M24)</f>
-        <v>53</v>
+        <f t="shared" si="0"/>
+        <v>56</v>
       </c>
       <c r="N25" s="4">
-        <f>M25-SUM(N2:N24)</f>
-        <v>48</v>
+        <f t="shared" si="0"/>
+        <v>51</v>
       </c>
       <c r="O25" s="4">
-        <f>N25-SUM(O2:O24)</f>
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="P25" s="4">
+        <f t="shared" si="0"/>
         <v>47</v>
       </c>
-      <c r="P25" s="4">
-        <f>O25-SUM(P2:P24)</f>
-        <v>44</v>
-      </c>
       <c r="Q25" s="4">
-        <f>P25-SUM(Q2:Q24)</f>
-        <v>34.5</v>
+        <f t="shared" si="0"/>
+        <v>37.5</v>
       </c>
       <c r="R25" s="4">
-        <f>Q25-SUM(R2:R24)</f>
-        <v>25.5</v>
+        <f t="shared" si="0"/>
+        <v>23.5</v>
       </c>
       <c r="S25" s="4">
-        <f>R25-SUM(S2:S24)</f>
-        <v>25.5</v>
+        <f t="shared" si="0"/>
+        <v>13.5</v>
       </c>
       <c r="T25" s="4">
-        <f>S25-SUM(T2:T24)</f>
-        <v>25.5</v>
+        <f t="shared" si="0"/>
+        <v>7.5</v>
       </c>
       <c r="U25" s="4">
-        <f>T25-SUM(U2:U24)</f>
-        <v>25.5</v>
+        <f t="shared" si="0"/>
+        <v>1.5</v>
       </c>
       <c r="V25" s="4">
-        <f>U25-SUM(V2:V24)</f>
-        <v>25.5</v>
+        <f t="shared" si="0"/>
+        <v>-1.5</v>
       </c>
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.25">
@@ -3340,64 +3387,64 @@
         <v>22</v>
       </c>
       <c r="B26" s="6">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="C26" s="6">
-        <v>94.05</v>
+        <v>96.9</v>
       </c>
       <c r="D26" s="6">
-        <v>89.1</v>
+        <v>91.8</v>
       </c>
       <c r="E26" s="6">
-        <v>84.15</v>
+        <v>86.7</v>
       </c>
       <c r="F26" s="6">
-        <v>79.2</v>
+        <v>81.599999999999994</v>
       </c>
       <c r="G26" s="6">
-        <v>74.25</v>
+        <v>76.5</v>
       </c>
       <c r="H26" s="6">
-        <v>69.3</v>
+        <v>71.400000000000006</v>
       </c>
       <c r="I26" s="6">
-        <v>64.349999999999994</v>
+        <v>66.3</v>
       </c>
       <c r="J26" s="6">
-        <v>59.4</v>
+        <v>61.2</v>
       </c>
       <c r="K26" s="6">
-        <v>54.45</v>
+        <v>56.100000000000101</v>
       </c>
       <c r="L26" s="6">
-        <v>49.5</v>
+        <v>51.000000000000099</v>
       </c>
       <c r="M26" s="6">
-        <v>44.55</v>
+        <v>45.900000000000098</v>
       </c>
       <c r="N26" s="6">
-        <v>39.6</v>
+        <v>40.800000000000097</v>
       </c>
       <c r="O26" s="6">
-        <v>34.65</v>
+        <v>35.700000000000102</v>
       </c>
       <c r="P26" s="6">
-        <v>29.7</v>
+        <v>30.600000000000101</v>
       </c>
       <c r="Q26" s="6">
-        <v>24.75</v>
+        <v>25.500000000000099</v>
       </c>
       <c r="R26" s="6">
-        <v>19.8</v>
+        <v>20.400000000000102</v>
       </c>
       <c r="S26" s="6">
-        <v>14.85</v>
+        <v>15.3000000000001</v>
       </c>
       <c r="T26" s="6">
-        <v>9.8999999999999098</v>
+        <v>10.200000000000101</v>
       </c>
       <c r="U26" s="6">
-        <v>4.9499999999998998</v>
+        <v>5.1000000000000902</v>
       </c>
       <c r="V26" s="6">
         <v>0</v>
@@ -3417,7 +3464,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7AEF5D5-9845-4510-B31C-B45C1A0563CA}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="N34" sqref="N34"/>
     </sheetView>
   </sheetViews>

</xml_diff>